<commit_message>
Added final changes to lab 4
</commit_message>
<xml_diff>
--- a/Lab 4 Stack Frame_Reeves.xlsx
+++ b/Lab 4 Stack Frame_Reeves.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Desktop\Assembly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Desktop\Assembly\Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24690" windowHeight="12525" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24690" windowHeight="12525" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="main1.c" sheetId="1" r:id="rId1"/>
     <sheet name="main2.c" sheetId="4" r:id="rId2"/>
     <sheet name="main3.c" sheetId="7" r:id="rId3"/>
     <sheet name="main4.c" sheetId="8" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
@@ -1359,7 +1360,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14:K21"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1962,6 +1963,616 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T33"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="1.28515625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="1.28515625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="14" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="15" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="13" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="13" customWidth="1"/>
+    <col min="14" max="14" width="1.28515625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="13" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="14" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="15" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" style="13" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" style="13" customWidth="1"/>
+    <col min="20" max="20" width="1.28515625" style="12" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="10"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="10"/>
+    </row>
+    <row r="2" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="10"/>
+    </row>
+    <row r="3" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="10"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="S5" s="18"/>
+    </row>
+    <row r="6" spans="1:20" ht="16.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="K8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="17"/>
+      <c r="Q8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T8" s="17"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="17"/>
+      <c r="O9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="T9" s="17"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R13" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="S13" s="18"/>
+    </row>
+    <row r="14" spans="1:20" ht="16.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="K15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="17"/>
+      <c r="K16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N16" s="17"/>
+      <c r="Q16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="T16" s="17"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N17" s="17"/>
+      <c r="O17" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="T17" s="17"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="I18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="K19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="31"/>
+      <c r="H20" s="17"/>
+      <c r="K20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20" s="17"/>
+      <c r="Q20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="T20" s="17"/>
+    </row>
+    <row r="21" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="18"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="R21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="S21" s="18"/>
+      <c r="T21" s="17"/>
+    </row>
+    <row r="22" spans="1:20" ht="16.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="29"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="Q23" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="26"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="O24" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="O25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="29"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="Q26" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="29"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="R27" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="S27" s="18"/>
+    </row>
+    <row r="28" spans="1:20" ht="16.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I28" s="29"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="29"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="Q29" s="32"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I30" s="29"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I31" s="29"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="Q31" s="30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I32" s="29"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+    </row>
+    <row r="33" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q33" s="33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="C567" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q14" sqref="Q14"/>
@@ -2310,616 +2921,6 @@
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N17" s="17"/>
-      <c r="O17" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="T17" s="17"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="I18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="K19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="31"/>
-      <c r="H20" s="17"/>
-      <c r="K20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N20" s="17"/>
-      <c r="Q20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="T20" s="17"/>
-    </row>
-    <row r="21" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L21" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="R21" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="S21" s="18"/>
-      <c r="T21" s="17"/>
-    </row>
-    <row r="22" spans="1:20" ht="16.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="I23" s="29"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="Q23" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="I24" s="26"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="O24" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q24" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="O25" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q25" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I26" s="29"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="Q26" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I27" s="29"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="R27" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="S27" s="18"/>
-    </row>
-    <row r="28" spans="1:20" ht="16.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="I28" s="29"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="21"/>
-      <c r="S28" s="21"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="I29" s="29"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="Q29" s="32"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="I30" s="29"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="I31" s="29"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="Q31" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="I32" s="29"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-    </row>
-    <row r="33" spans="17:17" x14ac:dyDescent="0.3">
-      <c r="Q33" s="33" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection password="C567" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T35"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="1.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="15" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="1.28515625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="14" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="15" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="13" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="13" customWidth="1"/>
-    <col min="14" max="14" width="1.28515625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="13" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="14" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" style="15" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" style="13" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" style="13" customWidth="1"/>
-    <col min="20" max="20" width="1.28515625" style="12" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="10"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="10"/>
-    </row>
-    <row r="2" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="10"/>
-    </row>
-    <row r="3" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="10"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="R5" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="S5" s="18"/>
-    </row>
-    <row r="6" spans="1:20" ht="16.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="17"/>
-      <c r="K8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" s="17"/>
-      <c r="Q8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T8" s="17"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" s="17"/>
-      <c r="O9" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T9" s="17"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="S13" s="18"/>
-    </row>
-    <row r="14" spans="1:20" ht="16.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="K15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q15" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="17"/>
-      <c r="K16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="N16" s="17"/>
-      <c r="Q16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="T16" s="17"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="17"/>
       <c r="K17" s="6" t="s">
         <v>54</v>
       </c>
@@ -3181,4 +3182,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>